<commit_message>
Compilato per valori tesi
</commit_message>
<xml_diff>
--- a/final_eigenvectors.xlsx
+++ b/final_eigenvectors.xlsx
@@ -457,58 +457,58 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8.421986066442642e-16</v>
+        <v>7.720153894239088e-16</v>
       </c>
       <c r="B2" t="n">
-        <v>-7.947634585102622e-08</v>
+        <v>-0.9999999999999989</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.9999999999999938</v>
+        <v>3.973817292551296e-08</v>
       </c>
       <c r="D2" t="n">
-        <v>-7.947634585102669e-08</v>
+        <v>-2.649211528367554e-08</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.64921152836755e-08</v>
+        <v>1.58952691702053e-08</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.9999999999999967</v>
+        <v>-3.973817292551311e-08</v>
       </c>
       <c r="C3" t="n">
-        <v>7.947634585102622e-08</v>
+        <v>-0.9999999999999991</v>
       </c>
       <c r="D3" t="n">
-        <v>3.506833688590627e-15</v>
+        <v>2.388943118032592e-15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.589526917020531e-08</v>
+        <v>1.324605764183779e-08</v>
       </c>
       <c r="B4" t="n">
-        <v>-2.16493489801906e-15</v>
+        <v>-2.649211528367546e-08</v>
       </c>
       <c r="C4" t="n">
-        <v>-7.947634585102661e-08</v>
+        <v>4.330927444391978e-15</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9999999999999969</v>
+        <v>0.9999999999999996</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.9999999999999996</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="B5" t="n">
-        <v>2.649211528367568e-08</v>
+        <v>1.754580430508887e-15</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.405485852517752e-31</v>
+        <v>1.589526917020529e-08</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.58952691702053e-08</v>
+        <v>-1.324605764183777e-08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>